<commit_message>
UPD test cases for Vereshaka
</commit_message>
<xml_diff>
--- a/Template_test_cases_vereshaka.xlsx
+++ b/Template_test_cases_vereshaka.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekaterina.andronova\Downloads\skillup1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="312" windowWidth="15132" windowHeight="7380" tabRatio="861" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="315" windowWidth="15135" windowHeight="7380" tabRatio="861" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="21" r:id="rId1"/>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <r>
       <t>How the tree directory is structured in Quality Center</t>
@@ -204,7 +209,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9">
     <font>
       <sz val="11"/>
@@ -404,6 +409,7 @@
   <cellStyles count="10">
     <cellStyle name="Hyperlink 3" xfId="1"/>
     <cellStyle name="Hyperlink 4" xfId="2"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2 18" xfId="3"/>
     <cellStyle name="Normal 4 3" xfId="4"/>
     <cellStyle name="Normal 8 3" xfId="5"/>
@@ -411,9 +417,178 @@
     <cellStyle name="Normal 8 5" xfId="7"/>
     <cellStyle name="Normal 8 6" xfId="8"/>
     <cellStyle name="Normal_webofscience checklist" xfId="9"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="60">
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color indexed="13"/>
@@ -768,7 +943,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="FSTA"/>
@@ -842,7 +1017,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="FSTA"/>
@@ -916,7 +1091,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="FSTA"/>
@@ -966,7 +1141,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="FSTA"/>
@@ -1016,9 +1191,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1056,9 +1231,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1090,9 +1265,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1124,9 +1300,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1299,16 +1476,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="106.6640625" customWidth="1"/>
+    <col min="1" max="1" width="106.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1438,28 +1615,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="9.109375" style="10"/>
-    <col min="3" max="3" width="9.6640625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="33.44140625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" style="11"/>
+    <col min="1" max="2" width="9.140625" style="10"/>
+    <col min="3" max="3" width="9.7109375" style="10" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="33.42578125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="11"/>
     <col min="7" max="7" width="62" style="10" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" style="10" customWidth="1"/>
-    <col min="9" max="9" width="63.5546875" style="10" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="10"/>
+    <col min="8" max="8" width="14.28515625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="63.5703125" style="10" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="12" customFormat="1" ht="66">
+    <row r="1" spans="1:19" s="12" customFormat="1" ht="63.75">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
@@ -1518,7 +1695,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="12" customFormat="1" ht="52.8">
+    <row r="2" spans="1:19" s="12" customFormat="1" ht="51">
       <c r="A2" s="5" t="s">
         <v>21</v>
       </c>
@@ -1582,7 +1759,7 @@
       <c r="R3" s="9"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:19" s="12" customFormat="1" ht="26.4">
+    <row r="4" spans="1:19" s="12" customFormat="1" ht="25.5">
       <c r="A4" s="5"/>
       <c r="B4" s="2"/>
       <c r="C4" s="23"/>
@@ -1611,16 +1788,32 @@
       <c r="R4" s="9"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:19" s="12" customFormat="1">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="19"/>
+    <row r="5" spans="1:19" s="12" customFormat="1" ht="51">
+      <c r="A5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="J5" s="13"/>
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
@@ -1633,15 +1826,21 @@
       <c r="S5" s="14"/>
     </row>
     <row r="6" spans="1:19" s="12" customFormat="1">
-      <c r="A6" s="17"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="19"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="3">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="J6" s="13"/>
       <c r="K6" s="15"/>
       <c r="L6" s="15"/>
@@ -1653,16 +1852,22 @@
       <c r="R6" s="16"/>
       <c r="S6" s="14"/>
     </row>
-    <row r="7" spans="1:19" s="12" customFormat="1">
-      <c r="A7" s="17"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
+    <row r="7" spans="1:19" s="12" customFormat="1" ht="15">
+      <c r="A7" s="5"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="3">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="J7" s="13"/>
       <c r="K7" s="15"/>
       <c r="L7" s="15"/>
@@ -1801,29 +2006,95 @@
       <c r="S13" s="14"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I4 G4:G6 I12:I13 G12:G13">
+  <conditionalFormatting sqref="I4 G4 I12:I13 G12:G13">
+    <cfRule type="cellIs" priority="109" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="110" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="111" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4 G4 I12:I13 G12:G13">
+    <cfRule type="cellIs" priority="106" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="107" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="108" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3 G3:G4">
+    <cfRule type="cellIs" priority="88" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="89" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="90" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3 G3:G4">
+    <cfRule type="cellIs" priority="85" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="86" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="87" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:P3">
+    <cfRule type="cellIs" priority="82" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="83" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="84" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:P3">
     <cfRule type="cellIs" priority="79" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="80" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="81" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4 G4:G6 I12:I13 G12:G13">
+    <cfRule type="cellIs" dxfId="49" priority="80" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="81" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2">
     <cfRule type="cellIs" priority="76" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="77" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="78" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3 G3:G4">
+    <cfRule type="cellIs" dxfId="47" priority="77" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="78" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="cellIs" priority="73" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="74" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="75" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4">
     <cfRule type="cellIs" priority="58" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
@@ -1834,7 +2105,7 @@
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3 G3:G4">
+  <conditionalFormatting sqref="I4">
     <cfRule type="cellIs" priority="55" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
@@ -1845,7 +2116,7 @@
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P2:P3">
+  <conditionalFormatting sqref="I3">
     <cfRule type="cellIs" priority="52" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
@@ -1856,7 +2127,7 @@
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P2:P3">
+  <conditionalFormatting sqref="I3">
     <cfRule type="cellIs" priority="49" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
@@ -1867,150 +2138,128 @@
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
-    <cfRule type="cellIs" priority="46" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="47" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="48" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
-    <cfRule type="cellIs" priority="43" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="44" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="45" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="G8:I11">
+    <cfRule type="cellIs" priority="34" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="35" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="36" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8:I11">
+    <cfRule type="cellIs" priority="31" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="32" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="33" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7 G7">
+    <cfRule type="cellIs" priority="28" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="29" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="30" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7 G7">
+    <cfRule type="cellIs" priority="25" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="26" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="27" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6 G6:G7">
+    <cfRule type="cellIs" priority="22" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="23" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="24" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6 G6:G7">
+    <cfRule type="cellIs" priority="19" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="20" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="21" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" priority="40" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="41" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="42" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" priority="16" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="17" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="18" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" priority="37" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="38" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="39" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" priority="34" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="35" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="36" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" priority="31" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="32" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="33" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" priority="28" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="29" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="30" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" priority="25" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="26" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="27" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3">
-    <cfRule type="cellIs" priority="22" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="23" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="24" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3">
-    <cfRule type="cellIs" priority="19" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="20" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="21" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" priority="13" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="14" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="15" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7">
+    <cfRule type="cellIs" priority="10" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="11" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="12" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7">
+    <cfRule type="cellIs" priority="7" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="8" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="9" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" priority="16" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="17" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" priority="4" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="5" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="6" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" priority="13" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="14" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="15" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G7:I11">
-    <cfRule type="cellIs" priority="4" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G7:I11">
     <cfRule type="cellIs" priority="1" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>

</xml_diff>